<commit_message>
issue #51 - updated template to use jx:params(formulaStrategy="BY_COLUMN")
</commit_message>
<xml_diff>
--- a/jxls-poi/src/test/resources/org/jxls/templatebasedtests/Issue51Test.xlsx
+++ b/jxls-poi/src/test/resources/org/jxls/templatebasedtests/Issue51Test.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\JobStuff\GitRepos\jxls\jxls-poi\src\test\resources\org\jxls\templatebasedtests\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7C1EEE-3C70-49CF-A19B-496E9474685B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="24195" windowHeight="13695"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -30,12 +24,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Felipe Queis</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -49,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="G6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -63,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="B7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="G7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -87,11 +81,12 @@
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
-          <t>jx:each(items="e.reportList" var="r" lastCell="G7" direction="RIGHT")</t>
+          <t xml:space="preserve">jx:each(items="e.reportList" var="r" lastCell="G7" direction="RIGHT")
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="G8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -101,7 +96,8 @@
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
-          <t>jx:each(items="dates" var="d" lastCell="G8" direction="RIGHT")</t>
+          <t>jx:each(items="dates" var="d" lastCell="G8" direction="RIGHT")
+jx:params(formulaStrategy="BY_COLUMN")</t>
         </r>
         <r>
           <rPr>
@@ -164,7 +160,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -323,7 +319,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -595,20 +591,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="5" width="10.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.1328125" style="3"/>
+    <col min="2" max="5" width="10.73046875" style="3" customWidth="1"/>
     <col min="6" max="6" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.7109375" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="3"/>
+    <col min="7" max="8" width="10.73046875" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.1328125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25"/>

</xml_diff>